<commit_message>
:memo: update journal de travail du 29 et du 30 avril
</commit_message>
<xml_diff>
--- a/frontend/Journal_de_Travail/Journal-de-Travail_FabreAntoine.xlsx
+++ b/frontend/Journal_de_Travail/Journal-de-Travail_FabreAntoine.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt52png\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt52png\Documents\GitHub\P_Web295\frontend\Journal_de_Travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D2F0C0-3981-4FCB-AE61-EA3C659C19D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F70A34A-2666-4CDA-AFF5-D6E7280B84A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -134,6 +134,18 @@
   </si>
   <si>
     <t>Maquette figma du frontend</t>
+  </si>
+  <si>
+    <t>Commencement de la page de recherche avec VueJs</t>
+  </si>
+  <si>
+    <t>finition de la page de recherche (juste du menu deroulant qui fait une requette quand on choisi quelque chose)</t>
+  </si>
+  <si>
+    <t>ajout d'une page de connexion pour se connecter et recevoir un jeton JWT</t>
+  </si>
+  <si>
+    <t>changement du backend pour que les jetons JWT soient envoyé dans les cookies et pas dans le headers</t>
   </si>
 </sst>
 </file>
@@ -1064,7 +1076,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1995,7 +2007,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2048,7 +2060,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 1 heurs 30 minutes</v>
+        <v>0 jours 4 heurs 30 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2063,15 +2075,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2155,15 +2167,23 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="str">
+      <c r="A9" s="16">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v/>
-      </c>
-      <c r="B9" s="50"/>
+        <v>18</v>
+      </c>
+      <c r="B9" s="50">
+        <v>45776</v>
+      </c>
       <c r="C9" s="51"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="36"/>
+      <c r="D9" s="52">
+        <v>45</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="56"/>
       <c r="M9" t="s">
         <v>4</v>
@@ -2175,16 +2195,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="str">
+    <row r="10" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="46"/>
+        <v>18</v>
+      </c>
+      <c r="B10" s="46">
+        <v>45777</v>
+      </c>
       <c r="C10" s="47"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="36"/>
+      <c r="D10" s="48">
+        <v>45</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>32</v>
+      </c>
       <c r="G10" s="55"/>
       <c r="M10" t="s">
         <v>5</v>
@@ -2197,15 +2225,23 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="str">
+      <c r="A11" s="16">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="51"/>
+        <v>18</v>
+      </c>
+      <c r="B11" s="50">
+        <v>45777</v>
+      </c>
+      <c r="C11" s="51">
+        <v>1</v>
+      </c>
       <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>33</v>
+      </c>
       <c r="G11" s="56"/>
       <c r="M11" t="s">
         <v>6</v>
@@ -2217,16 +2253,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="str">
+    <row r="12" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="46"/>
+        <v>18</v>
+      </c>
+      <c r="B12" s="46">
+        <v>45777</v>
+      </c>
       <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="36"/>
+      <c r="D12" s="48">
+        <v>30</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="G12" s="55"/>
       <c r="M12" t="s">
         <v>7</v>
@@ -8619,11 +8663,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8631,7 +8675,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8748,7 +8792,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>6.25E-2</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8762,6 +8806,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -8984,27 +9048,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9021,23 +9084,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>